<commit_message>
final changes of driver independent from driver version
</commit_message>
<xml_diff>
--- a/MDSi/bin/TestFiles/MDSiTestResult.xlsx
+++ b/MDSi/bin/TestFiles/MDSiTestResult.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>FileName</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>32297167</t>
+  </si>
+  <si>
+    <t>32297400</t>
+  </si>
+  <si>
+    <t>32297401</t>
+  </si>
+  <si>
+    <t>32297402</t>
   </si>
 </sst>
 </file>
@@ -577,7 +586,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -591,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -605,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Changes of 11th April 2022
</commit_message>
<xml_diff>
--- a/MDSi/bin/TestFiles/MDSiTestResult.xlsx
+++ b/MDSi/bin/TestFiles/MDSiTestResult.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Abhishek\ABHISHEK SHARMA\workspace\MDSi\src\TestFiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView tabRatio="614" windowHeight="9660" windowWidth="19812" xWindow="396" yWindow="516"/>
+    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" tabRatio="614"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>FileName</t>
   </si>
@@ -54,137 +49,19 @@
     <t>UPS</t>
   </si>
   <si>
-    <t>72004073</t>
-  </si>
-  <si>
-    <t>32001322</t>
-  </si>
-  <si>
-    <t>32265125</t>
-  </si>
-  <si>
-    <t>32288471</t>
-  </si>
-  <si>
-    <t>32288475</t>
-  </si>
-  <si>
-    <t>32288476</t>
-  </si>
-  <si>
-    <t>32291154</t>
-  </si>
-  <si>
-    <t>32291155</t>
-  </si>
-  <si>
-    <t>32291156</t>
-  </si>
-  <si>
-    <t>32291174</t>
-  </si>
-  <si>
-    <t>32291175</t>
-  </si>
-  <si>
-    <t>32291176</t>
-  </si>
-  <si>
-    <t>32291276</t>
-  </si>
-  <si>
-    <t>32291278</t>
-  </si>
-  <si>
-    <t>32291279</t>
-  </si>
-  <si>
-    <t>32294106</t>
-  </si>
-  <si>
-    <t>32294110</t>
-  </si>
-  <si>
-    <t>32294112</t>
-  </si>
-  <si>
-    <t>32294317</t>
-  </si>
-  <si>
-    <t>32294318</t>
-  </si>
-  <si>
-    <t>32294319</t>
-  </si>
-  <si>
-    <t>32294327</t>
-  </si>
-  <si>
-    <t>32294328</t>
-  </si>
-  <si>
-    <t>32294329</t>
-  </si>
-  <si>
-    <t>32294330</t>
-  </si>
-  <si>
-    <t>32294331</t>
-  </si>
-  <si>
-    <t>32294332</t>
-  </si>
-  <si>
-    <t>32294335</t>
-  </si>
-  <si>
-    <t>32294336</t>
-  </si>
-  <si>
-    <t>32294337</t>
-  </si>
-  <si>
-    <t>32295882</t>
-  </si>
-  <si>
-    <t>32295884</t>
-  </si>
-  <si>
-    <t>32295885</t>
-  </si>
-  <si>
-    <t>32296114</t>
-  </si>
-  <si>
-    <t>32296115</t>
-  </si>
-  <si>
-    <t>32296116</t>
-  </si>
-  <si>
-    <t>32297165</t>
-  </si>
-  <si>
-    <t>32297166</t>
-  </si>
-  <si>
-    <t>32297167</t>
-  </si>
-  <si>
     <t>32297400</t>
   </si>
   <si>
     <t>32297401</t>
   </si>
   <si>
-    <t>32297402</t>
+    <t>32339569</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -236,26 +113,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -272,10 +149,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -310,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,7 +222,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,7 +310,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -442,13 +319,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -458,7 +335,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -467,7 +344,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -476,7 +353,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -486,12 +363,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -522,7 +399,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -541,7 +418,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -553,18 +430,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.44140625" collapsed="true"/>
-    <col min="3" max="4" style="4" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -585,8 +462,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>50</v>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -599,8 +476,8 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>51</v>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -613,22 +490,16 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>52</v>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of 12th April 2022
</commit_message>
<xml_diff>
--- a/MDSi/bin/TestFiles/MDSiTestResult.xlsx
+++ b/MDSi/bin/TestFiles/MDSiTestResult.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" tabRatio="614"/>
+    <workbookView tabRatio="614" windowHeight="9660" windowWidth="19815" xWindow="390" yWindow="510"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>FileName</t>
   </si>
@@ -56,12 +56,31 @@
   </si>
   <si>
     <t>32339569</t>
+  </si>
+  <si>
+    <t>32341314</t>
+  </si>
+  <si>
+    <t>32341339</t>
+  </si>
+  <si>
+    <t>32341462</t>
+  </si>
+  <si>
+    <t>32341649</t>
+  </si>
+  <si>
+    <t>32341650</t>
+  </si>
+  <si>
+    <t>32341651</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -113,26 +132,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -149,10 +168,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -310,7 +329,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -319,13 +338,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -335,7 +354,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -344,7 +363,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -353,7 +372,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -363,12 +382,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -399,7 +418,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -418,7 +437,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -430,8 +449,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -439,9 +458,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="39.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="3" max="4" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -462,8 +481,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
+      <c r="B2" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -476,8 +495,8 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -490,8 +509,8 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
+      <c r="B4" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -499,7 +518,7 @@
       <c r="D4" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of Creation and tracking time
</commit_message>
<xml_diff>
--- a/MDSi/bin/TestFiles/MDSiTestResult.xlsx
+++ b/MDSi/bin/TestFiles/MDSiTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>FileName</t>
   </si>
@@ -209,6 +209,24 @@
   </si>
   <si>
     <t>32372252</t>
+  </si>
+  <si>
+    <t>32373945</t>
+  </si>
+  <si>
+    <t>32373946</t>
+  </si>
+  <si>
+    <t>32373947</t>
+  </si>
+  <si>
+    <t>32376214</t>
+  </si>
+  <si>
+    <t>32376215</t>
+  </si>
+  <si>
+    <t>32376217</t>
   </si>
 </sst>
 </file>
@@ -585,7 +603,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -617,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -631,7 +649,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -645,7 +663,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
CHanges of TrackingOrder issue for Headless browser
</commit_message>
<xml_diff>
--- a/MDSi/bin/TestFiles/MDSiTestResult.xlsx
+++ b/MDSi/bin/TestFiles/MDSiTestResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="94">
   <si>
     <t>FileName</t>
   </si>
@@ -227,6 +227,75 @@
   </si>
   <si>
     <t>32376217</t>
+  </si>
+  <si>
+    <t>32376658</t>
+  </si>
+  <si>
+    <t>32376659</t>
+  </si>
+  <si>
+    <t>32376660</t>
+  </si>
+  <si>
+    <t>32378671</t>
+  </si>
+  <si>
+    <t>32378672</t>
+  </si>
+  <si>
+    <t>32378673</t>
+  </si>
+  <si>
+    <t>32378878</t>
+  </si>
+  <si>
+    <t>32378879</t>
+  </si>
+  <si>
+    <t>32378880</t>
+  </si>
+  <si>
+    <t>32378887</t>
+  </si>
+  <si>
+    <t>32378888</t>
+  </si>
+  <si>
+    <t>32378889</t>
+  </si>
+  <si>
+    <t>32379639</t>
+  </si>
+  <si>
+    <t>32379640</t>
+  </si>
+  <si>
+    <t>32379641</t>
+  </si>
+  <si>
+    <t>32379863</t>
+  </si>
+  <si>
+    <t>32379864</t>
+  </si>
+  <si>
+    <t>32379865</t>
+  </si>
+  <si>
+    <t>32381542</t>
+  </si>
+  <si>
+    <t>32381543</t>
+  </si>
+  <si>
+    <t>32381731</t>
+  </si>
+  <si>
+    <t>32381732</t>
+  </si>
+  <si>
+    <t>32381733</t>
   </si>
 </sst>
 </file>
@@ -603,7 +672,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -635,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -649,7 +718,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -663,7 +732,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>

</xml_diff>